<commit_message>
update cac muc con thieu
</commit_message>
<xml_diff>
--- a/submit/PreliminarySchedule.xlsx
+++ b/submit/PreliminarySchedule.xlsx
@@ -563,8 +563,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.23713074266088738"/>
-          <c:y val="6.5118646751143233E-2"/>
+          <c:x val="0.27938131166853519"/>
+          <c:y val="0.13235414880070684"/>
           <c:w val="0.7471959143973067"/>
           <c:h val="0.93323767862350537"/>
         </c:manualLayout>
@@ -766,11 +766,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="101303808"/>
-        <c:axId val="101305344"/>
+        <c:axId val="80369536"/>
+        <c:axId val="80371072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101303808"/>
+        <c:axId val="80369536"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -788,12 +788,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400"/>
+              <a:defRPr sz="1200"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101305344"/>
+        <c:crossAx val="80371072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -801,7 +801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101305344"/>
+        <c:axId val="80371072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42650"/>
@@ -814,7 +814,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101303808"/>
+        <c:crossAx val="80369536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -1079,11 +1079,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="101583872"/>
-        <c:axId val="101593856"/>
+        <c:axId val="80383360"/>
+        <c:axId val="80086144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101583872"/>
+        <c:axId val="80383360"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1121,7 +1121,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101593856"/>
+        <c:crossAx val="80086144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1129,7 +1129,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101593856"/>
+        <c:axId val="80086144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42620"/>
@@ -1142,7 +1142,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101583872"/>
+        <c:crossAx val="80383360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -1487,11 +1487,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="101626624"/>
-        <c:axId val="101628160"/>
+        <c:axId val="80114816"/>
+        <c:axId val="80116352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101626624"/>
+        <c:axId val="80114816"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1505,7 +1505,7 @@
           <a:ln w="25400"/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="60000" vert="horz" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" vert="horz" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1514,7 +1514,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101628160"/>
+        <c:crossAx val="80116352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1522,7 +1522,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101628160"/>
+        <c:axId val="80116352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42620"/>
@@ -1535,7 +1535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101626624"/>
+        <c:crossAx val="80114816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="7"/>
@@ -2174,11 +2174,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="43454848"/>
-        <c:axId val="43456384"/>
+        <c:axId val="80149120"/>
+        <c:axId val="80216448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43454848"/>
+        <c:axId val="80149120"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2201,7 +2201,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43456384"/>
+        <c:crossAx val="80216448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2209,7 +2209,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43456384"/>
+        <c:axId val="80216448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42652"/>
@@ -2222,7 +2222,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43454848"/>
+        <c:crossAx val="80149120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="7"/>
@@ -2465,11 +2465,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="68987136"/>
-        <c:axId val="69935104"/>
+        <c:axId val="80254848"/>
+        <c:axId val="80256384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68987136"/>
+        <c:axId val="80254848"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2492,7 +2492,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69935104"/>
+        <c:crossAx val="80256384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2500,7 +2500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69935104"/>
+        <c:axId val="80256384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42650"/>
@@ -2513,7 +2513,250 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68987136"/>
+        <c:crossAx val="80254848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="7"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.27938131166853519"/>
+          <c:y val="0.13235414880070684"/>
+          <c:w val="0.7471959143973067"/>
+          <c:h val="0.93323767862350537"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>start date </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Set up hardware</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Find suitable hardware</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Set up electricity system</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Set up hardware</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Set up network(wifi, internet, LAN)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Test hardware system</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>42491</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42505</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42510</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42510</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42517</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>end date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Set up hardware</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Find suitable hardware</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Set up electricity system</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Set up hardware</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Set up network(wifi, internet, LAN)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Test hardware system</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="47068672"/>
+        <c:axId val="47070208"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="47068672"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="mm/dd/yy;@" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="25400"/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="47070208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="47070208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="42526"/>
+          <c:min val="42491"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="m/d;@" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="47068672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -2537,15 +2780,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>529318</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>112259</xdr:rowOff>
+      <xdr:colOff>116307</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>154099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>343581</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>112259</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>541484</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>31582</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2574,8 +2817,8 @@
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>214312</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>281609</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>187325</xdr:rowOff>
     </xdr:to>
@@ -2601,15 +2844,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>417514</xdr:colOff>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>466726</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>241789</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2665,15 +2908,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>394606</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>136071</xdr:rowOff>
+      <xdr:colOff>105103</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>113333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>136072</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>553308</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>120661</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2689,6 +2932,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>405848</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>224889</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>97886</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2986,8 +3261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH9" sqref="AH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3123,7 +3398,7 @@
         <v>42522</v>
       </c>
       <c r="C11" s="18">
-        <f>B11+D11-1</f>
+        <f t="shared" ref="C11:C27" si="1">B11+D11-1</f>
         <v>42528</v>
       </c>
       <c r="D11" s="28">
@@ -3138,7 +3413,7 @@
         <v>42522</v>
       </c>
       <c r="C12" s="10">
-        <f>B12+D12-1</f>
+        <f t="shared" si="1"/>
         <v>42528</v>
       </c>
       <c r="D12" s="30">
@@ -3153,7 +3428,7 @@
         <v>42522</v>
       </c>
       <c r="C13" s="10">
-        <f>B13+D13-1</f>
+        <f t="shared" si="1"/>
         <v>42528</v>
       </c>
       <c r="D13" s="31">
@@ -3168,7 +3443,7 @@
         <v>42529</v>
       </c>
       <c r="C14" s="10">
-        <f>B14+D14-1</f>
+        <f t="shared" si="1"/>
         <v>42529</v>
       </c>
       <c r="D14" s="31">
@@ -3183,7 +3458,7 @@
         <v>42530</v>
       </c>
       <c r="C15" s="10">
-        <f>B15+D15-1</f>
+        <f t="shared" si="1"/>
         <v>42534</v>
       </c>
       <c r="D15" s="31">
@@ -3198,7 +3473,7 @@
         <v>42535</v>
       </c>
       <c r="C16" s="10">
-        <f>B16+D16-1</f>
+        <f t="shared" si="1"/>
         <v>42535</v>
       </c>
       <c r="D16" s="31">
@@ -3213,7 +3488,7 @@
         <v>42536</v>
       </c>
       <c r="C17" s="10">
-        <f>B17+D17-1</f>
+        <f t="shared" si="1"/>
         <v>42542</v>
       </c>
       <c r="D17" s="31">
@@ -3228,7 +3503,7 @@
         <v>42543</v>
       </c>
       <c r="C18" s="10">
-        <f>B18+D18-1</f>
+        <f t="shared" si="1"/>
         <v>42546</v>
       </c>
       <c r="D18" s="31">
@@ -3243,7 +3518,7 @@
         <v>42547</v>
       </c>
       <c r="C19" s="10">
-        <f>B19+D19-1</f>
+        <f t="shared" si="1"/>
         <v>42553</v>
       </c>
       <c r="D19" s="31">
@@ -3258,7 +3533,7 @@
         <v>42554</v>
       </c>
       <c r="C20" s="10">
-        <f>B20+D20-1</f>
+        <f t="shared" si="1"/>
         <v>42555</v>
       </c>
       <c r="D20" s="31">
@@ -3273,7 +3548,7 @@
         <v>42556</v>
       </c>
       <c r="C21" s="10">
-        <f>B21+D21-1</f>
+        <f t="shared" si="1"/>
         <v>42556</v>
       </c>
       <c r="D21" s="31">
@@ -3288,7 +3563,7 @@
         <v>42557</v>
       </c>
       <c r="C22" s="10">
-        <f>B22+D22-1</f>
+        <f t="shared" si="1"/>
         <v>42559</v>
       </c>
       <c r="D22" s="31">
@@ -3303,7 +3578,7 @@
         <v>42560</v>
       </c>
       <c r="C23" s="10">
-        <f>B23+D23-1</f>
+        <f t="shared" si="1"/>
         <v>42564</v>
       </c>
       <c r="D23" s="31">
@@ -3318,7 +3593,7 @@
         <v>42565</v>
       </c>
       <c r="C24" s="10">
-        <f>B24+D24-1</f>
+        <f t="shared" si="1"/>
         <v>42569</v>
       </c>
       <c r="D24" s="31">
@@ -3333,7 +3608,7 @@
         <v>42570</v>
       </c>
       <c r="C25" s="10">
-        <f>B25+D25-1</f>
+        <f t="shared" si="1"/>
         <v>42570</v>
       </c>
       <c r="D25" s="31">
@@ -3348,7 +3623,7 @@
         <v>42571</v>
       </c>
       <c r="C26" s="10">
-        <f>B26+D26-1</f>
+        <f t="shared" si="1"/>
         <v>42615</v>
       </c>
       <c r="D26" s="31">
@@ -3363,7 +3638,7 @@
         <v>42617</v>
       </c>
       <c r="C27" s="24">
-        <f>B27+D27-1</f>
+        <f t="shared" si="1"/>
         <v>42618</v>
       </c>
       <c r="D27" s="34">
@@ -3397,7 +3672,7 @@
         <v>42531</v>
       </c>
       <c r="C31" s="18">
-        <f>B31+D31-1</f>
+        <f t="shared" ref="C31:C39" si="2">B31+D31-1</f>
         <v>42540</v>
       </c>
       <c r="D31" s="19">
@@ -3413,7 +3688,7 @@
         <v>42541</v>
       </c>
       <c r="C32" s="10">
-        <f>B32+D32-1</f>
+        <f t="shared" si="2"/>
         <v>42545</v>
       </c>
       <c r="D32" s="21">
@@ -3425,11 +3700,11 @@
         <v>23</v>
       </c>
       <c r="B33" s="13">
-        <f t="shared" ref="B33:B39" si="1">C32+1</f>
+        <f t="shared" ref="B33:B39" si="3">C32+1</f>
         <v>42546</v>
       </c>
       <c r="C33" s="10">
-        <f>B33+D33-1</f>
+        <f t="shared" si="2"/>
         <v>42555</v>
       </c>
       <c r="D33" s="21">
@@ -3441,11 +3716,11 @@
         <v>36</v>
       </c>
       <c r="B34" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>42556</v>
       </c>
       <c r="C34" s="10">
-        <f>B34+D34-1</f>
+        <f t="shared" si="2"/>
         <v>42615</v>
       </c>
       <c r="D34" s="21">
@@ -3457,11 +3732,11 @@
         <v>37</v>
       </c>
       <c r="B35" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>42616</v>
       </c>
       <c r="C35" s="10">
-        <f>B35+D35-1</f>
+        <f t="shared" si="2"/>
         <v>42625</v>
       </c>
       <c r="D35" s="21">
@@ -3473,11 +3748,11 @@
         <v>38</v>
       </c>
       <c r="B36" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>42626</v>
       </c>
       <c r="C36" s="10">
-        <f>B36+D36-1</f>
+        <f t="shared" si="2"/>
         <v>42635</v>
       </c>
       <c r="D36" s="21">
@@ -3489,11 +3764,11 @@
         <v>30</v>
       </c>
       <c r="B37" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>42636</v>
       </c>
       <c r="C37" s="10">
-        <f>B37+D37-1</f>
+        <f t="shared" si="2"/>
         <v>42637</v>
       </c>
       <c r="D37" s="21">
@@ -3505,11 +3780,11 @@
         <v>24</v>
       </c>
       <c r="B38" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>42638</v>
       </c>
       <c r="C38" s="10">
-        <f>B38+D38-1</f>
+        <f t="shared" si="2"/>
         <v>42640</v>
       </c>
       <c r="D38" s="21">
@@ -3521,11 +3796,11 @@
         <v>25</v>
       </c>
       <c r="B39" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>42641</v>
       </c>
       <c r="C39" s="24">
-        <f>B39+D39-1</f>
+        <f t="shared" si="2"/>
         <v>42647</v>
       </c>
       <c r="D39" s="25">
@@ -3560,7 +3835,7 @@
         <v>42531</v>
       </c>
       <c r="C43" s="10">
-        <f>B43+D43-1</f>
+        <f t="shared" ref="C43:C51" si="4">B43+D43-1</f>
         <v>42540</v>
       </c>
       <c r="D43" s="11">
@@ -3575,7 +3850,7 @@
         <v>42531</v>
       </c>
       <c r="C44" s="10">
-        <f>B44+D44-1</f>
+        <f t="shared" si="4"/>
         <v>42540</v>
       </c>
       <c r="D44" s="11">
@@ -3590,7 +3865,7 @@
         <v>42531</v>
       </c>
       <c r="C45" s="10">
-        <f>B45+D45-1</f>
+        <f t="shared" si="4"/>
         <v>42544</v>
       </c>
       <c r="D45" s="11">
@@ -3605,7 +3880,7 @@
         <v>42531</v>
       </c>
       <c r="C46" s="10">
-        <f>B46+D46-1</f>
+        <f t="shared" si="4"/>
         <v>42544</v>
       </c>
       <c r="D46" s="11">
@@ -3620,7 +3895,7 @@
         <v>42545</v>
       </c>
       <c r="C47" s="10">
-        <f>B47+D47-1</f>
+        <f t="shared" si="4"/>
         <v>42634</v>
       </c>
       <c r="D47" s="11">
@@ -3635,7 +3910,7 @@
         <v>42635</v>
       </c>
       <c r="C48" s="10">
-        <f>B48+D48-1</f>
+        <f t="shared" si="4"/>
         <v>42641</v>
       </c>
       <c r="D48" s="11">
@@ -3650,7 +3925,7 @@
         <v>42642</v>
       </c>
       <c r="C49" s="10">
-        <f>B49+D49-1</f>
+        <f t="shared" si="4"/>
         <v>42644</v>
       </c>
       <c r="D49" s="11">
@@ -3665,7 +3940,7 @@
         <v>42645</v>
       </c>
       <c r="C50" s="10">
-        <f>B50+D50-1</f>
+        <f t="shared" si="4"/>
         <v>42647</v>
       </c>
       <c r="D50" s="11">
@@ -3680,7 +3955,7 @@
         <v>42648</v>
       </c>
       <c r="C51" s="10">
-        <f>B51+D51-1</f>
+        <f t="shared" si="4"/>
         <v>42650</v>
       </c>
       <c r="D51" s="11">
@@ -3697,7 +3972,7 @@
       <c r="A53" s="4"/>
       <c r="B53" s="6"/>
       <c r="C53" s="7">
-        <f t="shared" ref="C53:C65" si="2">B53+D53-1</f>
+        <f t="shared" ref="C53:C65" si="5">B53+D53-1</f>
         <v>-1</v>
       </c>
       <c r="D53" s="5"/>
@@ -3706,7 +3981,7 @@
       <c r="A54" s="4"/>
       <c r="B54" s="6"/>
       <c r="C54" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="D54" s="5"/>
@@ -3715,7 +3990,7 @@
       <c r="A55" s="4"/>
       <c r="B55" s="6"/>
       <c r="C55" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="D55" s="5"/>
@@ -3724,7 +3999,7 @@
       <c r="A56" s="4"/>
       <c r="B56" s="6"/>
       <c r="C56" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="D56" s="5"/>
@@ -3733,7 +4008,7 @@
       <c r="A57" s="4"/>
       <c r="B57" s="6"/>
       <c r="C57" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="D57" s="5"/>
@@ -3742,7 +4017,7 @@
       <c r="A58" s="4"/>
       <c r="B58" s="6"/>
       <c r="C58" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="D58" s="5"/>
@@ -3751,7 +4026,7 @@
       <c r="A59" s="4"/>
       <c r="B59" s="6"/>
       <c r="C59" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="D59" s="5"/>
@@ -3760,7 +4035,7 @@
       <c r="A60" s="4"/>
       <c r="B60" s="6"/>
       <c r="C60" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="D60" s="5"/>
@@ -3769,7 +4044,7 @@
       <c r="A61" s="4"/>
       <c r="B61" s="6"/>
       <c r="C61" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="D61" s="5"/>
@@ -3778,7 +4053,7 @@
       <c r="A62" s="4"/>
       <c r="B62" s="6"/>
       <c r="C62" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="D62" s="5"/>
@@ -3787,7 +4062,7 @@
       <c r="A63" s="4"/>
       <c r="B63" s="6"/>
       <c r="C63" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="D63" s="5"/>
@@ -3796,7 +4071,7 @@
       <c r="A64" s="4"/>
       <c r="B64" s="6"/>
       <c r="C64" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="D64" s="5"/>
@@ -3805,7 +4080,7 @@
       <c r="A65" s="4"/>
       <c r="B65" s="6"/>
       <c r="C65" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="D65" s="5"/>
@@ -3814,7 +4089,7 @@
       <c r="A66" s="4"/>
       <c r="B66" s="6"/>
       <c r="C66" s="7">
-        <f t="shared" ref="C66:C97" si="3">B66+D66-1</f>
+        <f t="shared" ref="C66:C97" si="6">B66+D66-1</f>
         <v>-1</v>
       </c>
       <c r="D66" s="5"/>
@@ -3823,7 +4098,7 @@
       <c r="A67" s="4"/>
       <c r="B67" s="6"/>
       <c r="C67" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D67" s="5"/>
@@ -3832,7 +4107,7 @@
       <c r="A68" s="4"/>
       <c r="B68" s="6"/>
       <c r="C68" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D68" s="5"/>
@@ -3841,7 +4116,7 @@
       <c r="A69" s="4"/>
       <c r="B69" s="6"/>
       <c r="C69" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D69" s="5"/>
@@ -3850,7 +4125,7 @@
       <c r="A70" s="4"/>
       <c r="B70" s="6"/>
       <c r="C70" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D70" s="5"/>
@@ -3859,7 +4134,7 @@
       <c r="A71" s="4"/>
       <c r="B71" s="6"/>
       <c r="C71" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D71" s="5"/>
@@ -3868,7 +4143,7 @@
       <c r="A72" s="4"/>
       <c r="B72" s="6"/>
       <c r="C72" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D72" s="5"/>
@@ -3877,7 +4152,7 @@
       <c r="A73" s="4"/>
       <c r="B73" s="6"/>
       <c r="C73" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D73" s="5"/>
@@ -3886,7 +4161,7 @@
       <c r="A74" s="4"/>
       <c r="B74" s="6"/>
       <c r="C74" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D74" s="5"/>
@@ -3895,7 +4170,7 @@
       <c r="A75" s="4"/>
       <c r="B75" s="6"/>
       <c r="C75" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D75" s="5"/>
@@ -3904,7 +4179,7 @@
       <c r="A76" s="4"/>
       <c r="B76" s="6"/>
       <c r="C76" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D76" s="5"/>
@@ -3913,7 +4188,7 @@
       <c r="A77" s="4"/>
       <c r="B77" s="6"/>
       <c r="C77" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D77" s="5"/>
@@ -3922,7 +4197,7 @@
       <c r="A78" s="4"/>
       <c r="B78" s="6"/>
       <c r="C78" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D78" s="5"/>
@@ -3931,7 +4206,7 @@
       <c r="A79" s="4"/>
       <c r="B79" s="6"/>
       <c r="C79" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D79" s="5"/>
@@ -3940,7 +4215,7 @@
       <c r="A80" s="4"/>
       <c r="B80" s="6"/>
       <c r="C80" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D80" s="5"/>
@@ -3949,7 +4224,7 @@
       <c r="A81" s="4"/>
       <c r="B81" s="6"/>
       <c r="C81" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D81" s="5"/>
@@ -3958,7 +4233,7 @@
       <c r="A82" s="4"/>
       <c r="B82" s="6"/>
       <c r="C82" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D82" s="5"/>
@@ -3967,7 +4242,7 @@
       <c r="A83" s="4"/>
       <c r="B83" s="6"/>
       <c r="C83" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D83" s="5"/>
@@ -3976,7 +4251,7 @@
       <c r="A84" s="4"/>
       <c r="B84" s="6"/>
       <c r="C84" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D84" s="5"/>
@@ -3985,7 +4260,7 @@
       <c r="A85" s="4"/>
       <c r="B85" s="6"/>
       <c r="C85" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D85" s="5"/>
@@ -3994,7 +4269,7 @@
       <c r="A86" s="4"/>
       <c r="B86" s="6"/>
       <c r="C86" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D86" s="5"/>
@@ -4003,7 +4278,7 @@
       <c r="A87" s="4"/>
       <c r="B87" s="6"/>
       <c r="C87" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D87" s="5"/>
@@ -4012,7 +4287,7 @@
       <c r="A88" s="4"/>
       <c r="B88" s="6"/>
       <c r="C88" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D88" s="5"/>
@@ -4021,7 +4296,7 @@
       <c r="A89" s="4"/>
       <c r="B89" s="6"/>
       <c r="C89" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D89" s="5"/>
@@ -4030,7 +4305,7 @@
       <c r="A90" s="4"/>
       <c r="B90" s="6"/>
       <c r="C90" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D90" s="5"/>
@@ -4039,7 +4314,7 @@
       <c r="A91" s="4"/>
       <c r="B91" s="6"/>
       <c r="C91" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D91" s="5"/>
@@ -4048,7 +4323,7 @@
       <c r="A92" s="4"/>
       <c r="B92" s="6"/>
       <c r="C92" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D92" s="5"/>
@@ -4057,7 +4332,7 @@
       <c r="A93" s="4"/>
       <c r="B93" s="6"/>
       <c r="C93" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D93" s="5"/>
@@ -4066,7 +4341,7 @@
       <c r="A94" s="4"/>
       <c r="B94" s="6"/>
       <c r="C94" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D94" s="5"/>
@@ -4075,7 +4350,7 @@
       <c r="A95" s="4"/>
       <c r="B95" s="6"/>
       <c r="C95" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D95" s="2"/>
@@ -4084,7 +4359,7 @@
       <c r="A96" s="4"/>
       <c r="B96" s="6"/>
       <c r="C96" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D96" s="2"/>
@@ -4093,7 +4368,7 @@
       <c r="A97" s="4"/>
       <c r="B97" s="6"/>
       <c r="C97" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="D97" s="2"/>

</xml_diff>